<commit_message>
replace Wilkinson excel summary w/Taylor's updates
</commit_message>
<xml_diff>
--- a/book_summaries/Summary Politics and trade Policy, Joe Wilkinson.xlsx
+++ b/book_summaries/Summary Politics and trade Policy, Joe Wilkinson.xlsx
@@ -1,27 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10210"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10319"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/taylordunne/Documents/GitHub/gradualism/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D17D1CCC-774C-7345-88ED-77DB4F3E7F13}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="460" windowWidth="28560" windowHeight="17440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
-    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
-    <sheet name="Feuil3" sheetId="3" r:id="rId3"/>
+    <sheet name="Ch1 through Ch 4" sheetId="1" r:id="rId1"/>
+    <sheet name="Ch5 and Ch 6" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="210">
   <si>
     <t>Period</t>
   </si>
@@ -995,12 +995,204 @@
   <si>
     <t xml:space="preserve">H.R. 12591 passed 317-98 </t>
   </si>
+  <si>
+    <t>Politics and Trade Policy</t>
+  </si>
+  <si>
+    <t>Chapter 5: Trade Agreements in retrospect </t>
+  </si>
+  <si>
+    <t>5.1 – causal factors underlying the nature of support / opposition </t>
+  </si>
+  <si>
+    <t>• Directly related to problems facing the U.S. during the time of its existence, renewal, etc.</t>
+  </si>
+  <si>
+    <t>• 1939 – 1940: Depression</t>
+  </si>
+  <si>
+    <t>o Recovery measures = both side arguing its relationship to the depression:</t>
+  </si>
+  <si>
+    <t>o In favor of reducing tariffs: reciprocal nature would stimulate U.S. economy by liquidating agricultural surplus; restore employment (new deal component but sort of incompatible with the New Deal)</t>
+  </si>
+  <si>
+    <t>o Against reducing tariffs: Opening up trade would bring in too many imports and harm the industries involved; the protectionist policy of the 1920s brought in more trade than ever</t>
+  </si>
+  <si>
+    <t>• 1940 – 1945: WWII</t>
+  </si>
+  <si>
+    <t>o Success of the war and post war collaboration with allies </t>
+  </si>
+  <si>
+    <t>o In favor of reducing tariffs: Bipartisan support possible thanks to suspended individual judgement out of hope for end of war (main actor: Secretary Cordell Hull)</t>
+  </si>
+  <si>
+    <t>o Against reducing tariffs: Post war chaos is not the place to further reduce tariffs but rather a time to protect domestically</t>
+  </si>
+  <si>
+    <t>• Allies inability to cooperate leads to next stage: National Security</t>
+  </si>
+  <si>
+    <t>o U.S. influence on global trade (foreign policy strategy) – solidarity of the free world</t>
+  </si>
+  <si>
+    <t>o Cooperation between republican and democratic leaders </t>
+  </si>
+  <si>
+    <t>o 1948 inconsistency: “no-serious injury” policy vs. increased imports goal </t>
+  </si>
+  <si>
+    <t> Remaining opposition argued the harm to American industry</t>
+  </si>
+  <si>
+    <t>5.2 Changing patterns of opposition &amp; support</t>
+  </si>
+  <si>
+    <t>• Initially a partisan issue (Dems: for Reps: against)</t>
+  </si>
+  <si>
+    <t>• Slight divergence in 1940 and 1945</t>
+  </si>
+  <si>
+    <t>o Opposition by southern democrats after the textile industry moved south (out of New England)</t>
+  </si>
+  <si>
+    <t>o Rationale shifted from depression measure (American Exports) to international goodwill (American Imports)</t>
+  </si>
+  <si>
+    <t> Facilitated bipartisan protectionism coalition</t>
+  </si>
+  <si>
+    <t>5.3 Limitations of TAA</t>
+  </si>
+  <si>
+    <t>• Biggest flaw: ideally facilities trade without injuring any domestic industries</t>
+  </si>
+  <si>
+    <t>• No balance of trade within the act</t>
+  </si>
+  <si>
+    <t>• Avoids injury instead of providing means for shifts and adjustment mechanism</t>
+  </si>
+  <si>
+    <t>• Assumes trade is beneficial only if there is no injury </t>
+  </si>
+  <si>
+    <t> </t>
+  </si>
+  <si>
+    <t>Chapter 6: Trade Agreement Program in the Future (lots of if..then possibilities that may be helpful for modeling)</t>
+  </si>
+  <si>
+    <t>• Decreasing American import protection is beneficial for </t>
+  </si>
+  <si>
+    <t>o Making American economy more appealing than Soviet Union &amp; Soviet propaganda</t>
+  </si>
+  <si>
+    <t>o Stay on brand with European and developing economies’ views of the U.S. as leader of the free economy </t>
+  </si>
+  <si>
+    <t>o Benefit the American economy as well</t>
+  </si>
+  <si>
+    <t>• Prospects for political support </t>
+  </si>
+  <si>
+    <t>o For some time everyone will keep changes within the framework of the existing agreement</t>
+  </si>
+  <si>
+    <t>o Import restrictions will remain necessary</t>
+  </si>
+  <si>
+    <t>o National security purposes: will continue to receive bipartisan support as long as trade policy is subordinate to defense policy</t>
+  </si>
+  <si>
+    <t>• Renewing TAA</t>
+  </si>
+  <si>
+    <t>o Removal would be regression to smoot Hawley days </t>
+  </si>
+  <si>
+    <t>o Dependent on the status of liberal trade features vs. protection provisions</t>
+  </si>
+  <si>
+    <t>• Escape clause and peril point future:</t>
+  </si>
+  <si>
+    <t>o Wil remain as long as no-serious-injury remains important in either executive or legislative branch</t>
+  </si>
+  <si>
+    <t>o Escape clause exists only to allow for a period of adjustment but based on past/present experiences while peril point is based on predictions</t>
+  </si>
+  <si>
+    <t>o Could be interpreted as ighly protectionist</t>
+  </si>
+  <si>
+    <t>• Party support and opposition</t>
+  </si>
+  <si>
+    <t>o Depending on the movement of goods geographically and the results of the act long term</t>
+  </si>
+  <si>
+    <t>• Outside of congress</t>
+  </si>
+  <si>
+    <t>o Those adversely effected are a minority but they’re loud because collectivization is easier when things aren’t going your way</t>
+  </si>
+  <si>
+    <t>o 1953 survey of 825 “leading citizens” (44% business men): majority agree with lowering tariffs if reciprocated (which does not always manifest in the TAA) </t>
+  </si>
+  <si>
+    <t>o Additional indicators that business community is for liberalizing trade even if it means some businesses suffer</t>
+  </si>
+  <si>
+    <t>o Burden of proof moves from domestic protectionists to those who prefer international cooperation </t>
+  </si>
+  <si>
+    <t>• Need for a new Liberal Trade approach:</t>
+  </si>
+  <si>
+    <t>o US Council on the International Chamber of Commerce</t>
+  </si>
+  <si>
+    <t> TAA should express general national interests</t>
+  </si>
+  <si>
+    <t> Permit trade to replace foreign aid</t>
+  </si>
+  <si>
+    <t> Provide basis for negotiation promoting U.S. exports</t>
+  </si>
+  <si>
+    <t> Avoid inefficient use of U.S. resources</t>
+  </si>
+  <si>
+    <t> Avoid serious injury</t>
+  </si>
+  <si>
+    <t> Afford easier access to resources used by Americans</t>
+  </si>
+  <si>
+    <t> Encourage investment abroad</t>
+  </si>
+  <si>
+    <t> Strengthen free world in the fight against communism </t>
+  </si>
+  <si>
+    <t>o More explanation of consumer benefit</t>
+  </si>
+  <si>
+    <t>• Cordell Hull and William Clayton – credited with success of Roosevelt and Truman admin securing congressional support for TAA extensions up to 1948</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="6">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1040,6 +1232,19 @@
     <font>
       <i/>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1098,11 +1303,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -1159,6 +1361,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1505,574 +1713,574 @@
   </sheetPr>
   <dimension ref="A1:S19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="131" zoomScaleNormal="131" workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="12.5" style="3" customWidth="1"/>
-    <col min="2" max="2" width="11.5" style="3" customWidth="1"/>
-    <col min="3" max="3" width="46.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="46.6640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="39.33203125" style="3" customWidth="1"/>
-    <col min="7" max="7" width="37.5" style="3" customWidth="1"/>
-    <col min="8" max="11" width="44.83203125" style="3" customWidth="1"/>
-    <col min="12" max="14" width="47" style="3" customWidth="1"/>
-    <col min="15" max="15" width="59.33203125" style="3" customWidth="1"/>
-    <col min="16" max="16" width="35" style="17" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="25.33203125" style="3" customWidth="1"/>
-    <col min="18" max="18" width="25.83203125" style="3" customWidth="1"/>
-    <col min="19" max="19" width="34.6640625" style="3" customWidth="1"/>
-    <col min="20" max="20" width="33.33203125" style="3" customWidth="1"/>
-    <col min="21" max="21" width="44.5" style="3" customWidth="1"/>
-    <col min="22" max="16384" width="10.83203125" style="3"/>
+    <col min="1" max="1" width="12.5" style="2" customWidth="1"/>
+    <col min="2" max="2" width="11.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="46.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="46.6640625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="39.33203125" style="2" customWidth="1"/>
+    <col min="7" max="7" width="37.5" style="2" customWidth="1"/>
+    <col min="8" max="11" width="44.83203125" style="2" customWidth="1"/>
+    <col min="12" max="14" width="47" style="2" customWidth="1"/>
+    <col min="15" max="15" width="59.33203125" style="2" customWidth="1"/>
+    <col min="16" max="16" width="35" style="16" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="25.33203125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="25.83203125" style="2" customWidth="1"/>
+    <col min="19" max="19" width="34.6640625" style="2" customWidth="1"/>
+    <col min="20" max="20" width="33.33203125" style="2" customWidth="1"/>
+    <col min="21" max="21" width="44.5" style="2" customWidth="1"/>
+    <col min="22" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1" t="s">
+      <c r="D1" s="21"/>
+      <c r="E1" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="F1" s="21"/>
+      <c r="G1" s="21" t="s">
         <v>9</v>
       </c>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="2" t="s">
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="2"/>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2"/>
-      <c r="P1" s="2" t="s">
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
+      <c r="P1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="Q1" s="4"/>
-      <c r="R1" s="4"/>
-      <c r="S1" s="4"/>
-    </row>
-    <row r="2" spans="1:19" s="7" customFormat="1">
-      <c r="A2" s="5"/>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5">
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
+      <c r="S1" s="3"/>
+    </row>
+    <row r="2" spans="1:19" s="6" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4">
         <v>1934</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="4">
         <v>1937</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="4">
         <v>1940</v>
       </c>
-      <c r="F2" s="5">
+      <c r="F2" s="4">
         <v>1943</v>
       </c>
-      <c r="G2" s="5">
+      <c r="G2" s="4">
         <v>1945</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2" s="4">
         <v>1948</v>
       </c>
-      <c r="I2" s="5">
+      <c r="I2" s="4">
         <v>1949</v>
       </c>
-      <c r="J2" s="5">
+      <c r="J2" s="4">
         <v>1951</v>
       </c>
-      <c r="K2" s="5">
+      <c r="K2" s="4">
         <v>1953</v>
       </c>
-      <c r="L2" s="6">
+      <c r="L2" s="5">
         <v>1954</v>
       </c>
-      <c r="M2" s="6">
+      <c r="M2" s="5">
         <v>1955</v>
       </c>
-      <c r="N2" s="6">
+      <c r="N2" s="5">
         <v>1958</v>
       </c>
-      <c r="P2" s="8" t="s">
+      <c r="P2" s="7" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="11" customFormat="1" ht="165">
-      <c r="A3" s="9" t="s">
+    <row r="3" spans="1:19" s="10" customFormat="1" ht="165" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="B3" s="9"/>
-      <c r="C3" s="9" t="s">
+      <c r="B3" s="8"/>
+      <c r="C3" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="8" t="s">
         <v>127</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="G3" s="9" t="s">
+      <c r="G3" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="H3" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="I3" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="J3" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="9" t="s">
         <v>89</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="L3" s="9" t="s">
         <v>114</v>
       </c>
-      <c r="M3" s="10" t="s">
+      <c r="M3" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="N3" s="10" t="s">
+      <c r="N3" s="9" t="s">
         <v>123</v>
       </c>
-      <c r="O3" s="11" t="s">
+      <c r="O3" s="10" t="s">
         <v>99</v>
       </c>
-      <c r="P3" s="12" t="s">
+      <c r="P3" s="11" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="105">
-      <c r="A4" s="13" t="s">
+    <row r="4" spans="1:19" ht="105" x14ac:dyDescent="0.2">
+      <c r="A4" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="14" t="s">
+      <c r="B4" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="14" t="s">
         <v>129</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="14" t="s">
         <v>48</v>
       </c>
-      <c r="H4" s="14" t="s">
+      <c r="H4" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="I4" s="14" t="s">
+      <c r="I4" s="13" t="s">
         <v>76</v>
       </c>
-      <c r="J4" s="14" t="s">
+      <c r="J4" s="13" t="s">
         <v>82</v>
       </c>
-      <c r="K4" s="14" t="s">
+      <c r="K4" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="L4" s="14" t="s">
+      <c r="L4" s="13" t="s">
         <v>107</v>
       </c>
-      <c r="M4" s="14" t="s">
+      <c r="M4" s="13" t="s">
         <v>116</v>
       </c>
-      <c r="O4" s="16" t="s">
+      <c r="O4" s="15" t="s">
         <v>130</v>
       </c>
-      <c r="P4" s="16" t="s">
+      <c r="P4" s="15" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="90">
-      <c r="A5" s="13"/>
-      <c r="B5" s="14" t="s">
+    <row r="5" spans="1:19" ht="90" x14ac:dyDescent="0.2">
+      <c r="A5" s="12"/>
+      <c r="B5" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>132</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="E5" s="14" t="s">
+      <c r="E5" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="F5" s="14" t="s">
+      <c r="F5" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="G5" s="14" t="s">
+      <c r="G5" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="H5" s="14" t="s">
+      <c r="H5" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="I5" s="14" t="s">
+      <c r="I5" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="J5" s="14" t="s">
+      <c r="J5" s="13" t="s">
         <v>83</v>
       </c>
-      <c r="K5" s="14" t="s">
+      <c r="K5" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="L5" s="14" t="s">
+      <c r="L5" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="M5" s="14" t="s">
+      <c r="M5" s="13" t="s">
         <v>118</v>
       </c>
-      <c r="P5" s="16" t="s">
+      <c r="P5" s="15" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="90">
-      <c r="A6" s="13" t="s">
+    <row r="6" spans="1:19" ht="90" x14ac:dyDescent="0.2">
+      <c r="A6" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="B6" s="13"/>
-      <c r="C6" s="14" t="s">
+      <c r="B6" s="12"/>
+      <c r="C6" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="14" t="s">
+      <c r="D6" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="14" t="s">
+      <c r="E6" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="14" t="s">
+      <c r="F6" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="G6" s="14" t="s">
+      <c r="G6" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="H6" s="14" t="s">
+      <c r="H6" s="13" t="s">
         <v>69</v>
       </c>
-      <c r="I6" s="14" t="s">
+      <c r="I6" s="13" t="s">
         <v>80</v>
       </c>
-      <c r="J6" s="14" t="s">
+      <c r="J6" s="13" t="s">
         <v>84</v>
       </c>
-      <c r="K6" s="14" t="s">
+      <c r="K6" s="13" t="s">
         <v>93</v>
       </c>
-      <c r="L6" s="14" t="s">
+      <c r="L6" s="13" t="s">
         <v>109</v>
       </c>
-      <c r="M6" s="14" t="s">
+      <c r="M6" s="13" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="180">
-      <c r="A7" s="13" t="s">
+    <row r="7" spans="1:19" ht="180" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="14" t="s">
+      <c r="E7" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="F7" s="14" t="s">
+      <c r="F7" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="14" t="s">
+      <c r="G7" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="H7" s="14" t="s">
+      <c r="H7" s="13" t="s">
         <v>71</v>
       </c>
-      <c r="I7" s="14" t="s">
+      <c r="I7" s="13" t="s">
         <v>75</v>
       </c>
-      <c r="J7" s="14" t="s">
+      <c r="J7" s="13" t="s">
         <v>92</v>
       </c>
-      <c r="K7" s="14" t="s">
+      <c r="K7" s="13" t="s">
         <v>96</v>
       </c>
-      <c r="L7" s="14" t="s">
+      <c r="L7" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="M7" s="14" t="s">
+      <c r="M7" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="P7" s="16" t="s">
+      <c r="P7" s="15" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="135">
-      <c r="A8" s="13"/>
-      <c r="B8" s="14" t="s">
+    <row r="8" spans="1:19" ht="135" x14ac:dyDescent="0.2">
+      <c r="A8" s="12"/>
+      <c r="B8" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="14" t="s">
+      <c r="C8" s="13" t="s">
         <v>137</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="E8" s="14" t="s">
+      <c r="E8" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="F8" s="14" t="s">
+      <c r="F8" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="13" t="s">
         <v>70</v>
       </c>
-      <c r="I8" s="14" t="s">
+      <c r="I8" s="13" t="s">
         <v>77</v>
       </c>
-      <c r="J8" s="14" t="s">
+      <c r="J8" s="13" t="s">
         <v>85</v>
       </c>
-      <c r="K8" s="14" t="s">
+      <c r="K8" s="13" t="s">
         <v>97</v>
       </c>
-      <c r="L8" s="14" t="s">
+      <c r="L8" s="13" t="s">
         <v>111</v>
       </c>
-      <c r="M8" s="14" t="s">
+      <c r="M8" s="13" t="s">
         <v>120</v>
       </c>
-      <c r="P8" s="16" t="s">
+      <c r="P8" s="15" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="210">
-      <c r="A9" s="13" t="s">
+    <row r="9" spans="1:19" ht="210" x14ac:dyDescent="0.2">
+      <c r="A9" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="B9" s="13"/>
-      <c r="C9" s="14" t="s">
+      <c r="B9" s="12"/>
+      <c r="C9" s="13" t="s">
         <v>140</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="13" t="s">
         <v>141</v>
       </c>
-      <c r="E9" s="14" t="s">
+      <c r="E9" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="14" t="s">
+      <c r="F9" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="14" t="s">
+      <c r="G9" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="H9" s="14" t="s">
+      <c r="H9" s="13" t="s">
         <v>72</v>
       </c>
-      <c r="I9" s="14" t="s">
+      <c r="I9" s="13" t="s">
         <v>78</v>
       </c>
-      <c r="J9" s="14" t="s">
+      <c r="J9" s="13" t="s">
         <v>86</v>
       </c>
-      <c r="K9" s="14" t="s">
+      <c r="K9" s="13" t="s">
         <v>98</v>
       </c>
-      <c r="L9" s="14" t="s">
+      <c r="L9" s="13" t="s">
         <v>112</v>
       </c>
-      <c r="M9" s="14" t="s">
+      <c r="M9" s="13" t="s">
         <v>121</v>
       </c>
-      <c r="P9" s="16" t="s">
+      <c r="P9" s="15" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="10" spans="1:19" ht="60">
-      <c r="A10" s="13" t="s">
+    <row r="10" spans="1:19" ht="60" x14ac:dyDescent="0.2">
+      <c r="A10" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="13"/>
-      <c r="C10" s="14" t="s">
+      <c r="B10" s="12"/>
+      <c r="C10" s="13" t="s">
         <v>143</v>
       </c>
-      <c r="D10" s="14" t="s">
+      <c r="D10" s="13" t="s">
         <v>144</v>
       </c>
-      <c r="E10" s="14" t="s">
+      <c r="E10" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="13" t="s">
         <v>73</v>
       </c>
-      <c r="I10" s="14" t="s">
+      <c r="I10" s="13" t="s">
         <v>81</v>
       </c>
-      <c r="J10" s="14" t="s">
+      <c r="J10" s="13" t="s">
         <v>88</v>
       </c>
-      <c r="K10" s="14" t="s">
+      <c r="K10" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="L10" s="14" t="s">
+      <c r="L10" s="13" t="s">
         <v>113</v>
       </c>
-      <c r="M10" s="14" t="s">
+      <c r="M10" s="13" t="s">
         <v>122</v>
       </c>
-      <c r="P10" s="17" t="s">
+      <c r="P10" s="16" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="30">
-      <c r="K14" s="18" t="s">
+    <row r="14" spans="1:19" ht="30" x14ac:dyDescent="0.2">
+      <c r="K14" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="L14" s="18" t="s">
+      <c r="L14" s="17" t="s">
         <v>16</v>
       </c>
-      <c r="M14" s="18" t="s">
+      <c r="M14" s="17" t="s">
         <v>21</v>
       </c>
-      <c r="N14" s="18" t="s">
+      <c r="N14" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="O14" s="18" t="s">
+      <c r="O14" s="17" t="s">
         <v>59</v>
       </c>
-      <c r="P14" s="19" t="s">
+      <c r="P14" s="18" t="s">
         <v>63</v>
       </c>
-      <c r="Q14" s="18" t="s">
+      <c r="Q14" s="17" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="15" spans="1:19">
-      <c r="K15" s="11" t="s">
+    <row r="15" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="K15" s="10" t="s">
         <v>57</v>
       </c>
-      <c r="L15" s="11" t="s">
+      <c r="L15" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="M15" s="11" t="s">
+      <c r="M15" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="N15" s="20">
+      <c r="N15" s="19">
         <v>1817</v>
       </c>
-      <c r="O15" s="11" t="s">
+      <c r="O15" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="P15" s="12" t="s">
+      <c r="P15" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="Q15" s="21">
+      <c r="Q15" s="20">
         <v>1953</v>
       </c>
     </row>
-    <row r="16" spans="1:19" ht="75">
-      <c r="K16" s="11" t="s">
+    <row r="16" spans="1:19" ht="75" x14ac:dyDescent="0.2">
+      <c r="K16" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="L16" s="11" t="s">
+      <c r="L16" s="10" t="s">
         <v>17</v>
       </c>
-      <c r="M16" s="11" t="s">
+      <c r="M16" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="N16" s="11" t="s">
+      <c r="N16" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="O16" s="11" t="s">
+      <c r="O16" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="P16" s="12" t="s">
+      <c r="P16" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="Q16" s="11" t="s">
+      <c r="Q16" s="10" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="17" spans="11:17" ht="30">
-      <c r="K17" s="11" t="s">
+    <row r="17" spans="11:17" ht="30" x14ac:dyDescent="0.2">
+      <c r="K17" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="L17" s="11" t="s">
+      <c r="L17" s="10" t="s">
         <v>94</v>
       </c>
-      <c r="M17" s="11" t="s">
+      <c r="M17" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="N17" s="11" t="s">
+      <c r="N17" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="O17" s="11" t="s">
+      <c r="O17" s="10" t="s">
         <v>100</v>
       </c>
-      <c r="P17" s="12" t="s">
+      <c r="P17" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="Q17" s="11" t="s">
+      <c r="Q17" s="10" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="18" spans="11:17" ht="90">
-      <c r="K18" s="11" t="s">
+    <row r="18" spans="11:17" ht="90" x14ac:dyDescent="0.2">
+      <c r="K18" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="L18" s="11" t="s">
+      <c r="L18" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="M18" s="11"/>
-      <c r="N18" s="11"/>
-      <c r="O18" s="12" t="s">
+      <c r="M18" s="10"/>
+      <c r="N18" s="10"/>
+      <c r="O18" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="P18" s="12" t="s">
+      <c r="P18" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="Q18" s="11" t="s">
+      <c r="Q18" s="10" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="19" spans="11:17" ht="30">
-      <c r="K19" s="11" t="s">
+    <row r="19" spans="11:17" ht="30" x14ac:dyDescent="0.2">
+      <c r="K19" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="11"/>
-      <c r="O19" s="11"/>
-      <c r="P19" s="12" t="s">
+      <c r="L19" s="10"/>
+      <c r="M19" s="10"/>
+      <c r="N19" s="10"/>
+      <c r="O19" s="10"/>
+      <c r="P19" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="Q19" s="11" t="s">
+      <c r="Q19" s="10" t="s">
         <v>102</v>
       </c>
     </row>
@@ -2094,24 +2302,1854 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:M166"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A32" sqref="A32"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="16384" width="10.83203125" style="23"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="22" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A2" s="22" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="22" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="22" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="22" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A6" s="22" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A7" s="22" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="22" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A9" s="22" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="22" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="22" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A12" s="22" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="22" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="22" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A15" s="22" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A16" s="22" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A17" s="22" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" s="23" customFormat="1" x14ac:dyDescent="0.2"/>
+    <row r="19" spans="1:1" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A19" s="22" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A20" s="22" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="22" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="22" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="22" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A24" s="22" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A25" s="22" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A26" s="22" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A27" s="22" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="22" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A29" s="22" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" s="23" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="22" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="24" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="24" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="24" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="24" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="24" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="24" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="24" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="24" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="24" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="24" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="24" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="24" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="24" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="24" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="24" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="24" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="47" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="24" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="48" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="24" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="49" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="24" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="24" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="51" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="24" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="24" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="24" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="54" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="24" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="55" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="24" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="24" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="57" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="24" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="24" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="24" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="60" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="24" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="61" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="24" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="24" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="63" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="24" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="64" spans="1:1" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="24" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" s="23" customFormat="1" ht="19" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="24" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A66" s="24"/>
+      <c r="B66" s="24"/>
+      <c r="C66" s="24"/>
+      <c r="D66" s="24"/>
+      <c r="E66" s="24"/>
+      <c r="F66" s="24"/>
+      <c r="G66" s="24"/>
+      <c r="H66" s="24"/>
+      <c r="I66" s="24"/>
+      <c r="J66" s="24"/>
+      <c r="K66" s="24"/>
+      <c r="L66" s="24"/>
+      <c r="M66" s="24"/>
+    </row>
+    <row r="67" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A67" s="24"/>
+      <c r="B67" s="24"/>
+      <c r="C67" s="24"/>
+      <c r="D67" s="24"/>
+      <c r="E67" s="24"/>
+      <c r="F67" s="24"/>
+      <c r="G67" s="24"/>
+      <c r="H67" s="24"/>
+      <c r="I67" s="24"/>
+      <c r="J67" s="24"/>
+      <c r="K67" s="24"/>
+      <c r="L67" s="24"/>
+      <c r="M67" s="24"/>
+    </row>
+    <row r="68" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A68" s="24"/>
+      <c r="B68" s="24"/>
+      <c r="C68" s="24"/>
+      <c r="D68" s="24"/>
+      <c r="E68" s="24"/>
+      <c r="F68" s="24"/>
+      <c r="G68" s="24"/>
+      <c r="H68" s="24"/>
+      <c r="I68" s="24"/>
+      <c r="J68" s="24"/>
+      <c r="K68" s="24"/>
+      <c r="L68" s="24"/>
+      <c r="M68" s="24"/>
+    </row>
+    <row r="69" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A69" s="24"/>
+      <c r="B69" s="24"/>
+      <c r="C69" s="24"/>
+      <c r="D69" s="24"/>
+      <c r="E69" s="24"/>
+      <c r="F69" s="24"/>
+      <c r="G69" s="24"/>
+      <c r="H69" s="24"/>
+      <c r="I69" s="24"/>
+      <c r="J69" s="24"/>
+      <c r="K69" s="24"/>
+      <c r="L69" s="24"/>
+      <c r="M69" s="24"/>
+    </row>
+    <row r="70" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A70" s="24"/>
+      <c r="B70" s="24"/>
+      <c r="C70" s="24"/>
+      <c r="D70" s="24"/>
+      <c r="E70" s="24"/>
+      <c r="F70" s="24"/>
+      <c r="G70" s="24"/>
+      <c r="H70" s="24"/>
+      <c r="I70" s="24"/>
+      <c r="J70" s="24"/>
+      <c r="K70" s="24"/>
+      <c r="L70" s="24"/>
+      <c r="M70" s="24"/>
+    </row>
+    <row r="71" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A71" s="24"/>
+      <c r="B71" s="24"/>
+      <c r="C71" s="24"/>
+      <c r="D71" s="24"/>
+      <c r="E71" s="24"/>
+      <c r="F71" s="24"/>
+      <c r="G71" s="24"/>
+      <c r="H71" s="24"/>
+      <c r="I71" s="24"/>
+      <c r="J71" s="24"/>
+      <c r="K71" s="24"/>
+      <c r="L71" s="24"/>
+      <c r="M71" s="24"/>
+    </row>
+    <row r="72" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A72" s="24"/>
+      <c r="B72" s="24"/>
+      <c r="C72" s="24"/>
+      <c r="D72" s="24"/>
+      <c r="E72" s="24"/>
+      <c r="F72" s="24"/>
+      <c r="G72" s="24"/>
+      <c r="H72" s="24"/>
+      <c r="I72" s="24"/>
+      <c r="J72" s="24"/>
+      <c r="K72" s="24"/>
+      <c r="L72" s="24"/>
+      <c r="M72" s="24"/>
+    </row>
+    <row r="73" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A73" s="24"/>
+      <c r="B73" s="24"/>
+      <c r="C73" s="24"/>
+      <c r="D73" s="24"/>
+      <c r="E73" s="24"/>
+      <c r="F73" s="24"/>
+      <c r="G73" s="24"/>
+      <c r="H73" s="24"/>
+      <c r="I73" s="24"/>
+      <c r="J73" s="24"/>
+      <c r="K73" s="24"/>
+      <c r="L73" s="24"/>
+      <c r="M73" s="24"/>
+    </row>
+    <row r="74" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A74" s="24"/>
+      <c r="B74" s="24"/>
+      <c r="C74" s="24"/>
+      <c r="D74" s="24"/>
+      <c r="E74" s="24"/>
+      <c r="F74" s="24"/>
+      <c r="G74" s="24"/>
+      <c r="H74" s="24"/>
+      <c r="I74" s="24"/>
+      <c r="J74" s="24"/>
+      <c r="K74" s="24"/>
+      <c r="L74" s="24"/>
+      <c r="M74" s="24"/>
+    </row>
+    <row r="75" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A75" s="24"/>
+      <c r="B75" s="24"/>
+      <c r="C75" s="24"/>
+      <c r="D75" s="24"/>
+      <c r="E75" s="24"/>
+      <c r="F75" s="24"/>
+      <c r="G75" s="24"/>
+      <c r="H75" s="24"/>
+      <c r="I75" s="24"/>
+      <c r="J75" s="24"/>
+      <c r="K75" s="24"/>
+      <c r="L75" s="24"/>
+      <c r="M75" s="24"/>
+    </row>
+    <row r="76" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A76" s="24"/>
+      <c r="B76" s="24"/>
+      <c r="C76" s="24"/>
+      <c r="D76" s="24"/>
+      <c r="E76" s="24"/>
+      <c r="F76" s="24"/>
+      <c r="G76" s="24"/>
+      <c r="H76" s="24"/>
+      <c r="I76" s="24"/>
+      <c r="J76" s="24"/>
+      <c r="K76" s="24"/>
+      <c r="L76" s="24"/>
+      <c r="M76" s="24"/>
+    </row>
+    <row r="77" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A77" s="24"/>
+      <c r="B77" s="24"/>
+      <c r="C77" s="24"/>
+      <c r="D77" s="24"/>
+      <c r="E77" s="24"/>
+      <c r="F77" s="24"/>
+      <c r="G77" s="24"/>
+      <c r="H77" s="24"/>
+      <c r="I77" s="24"/>
+      <c r="J77" s="24"/>
+      <c r="K77" s="24"/>
+      <c r="L77" s="24"/>
+      <c r="M77" s="24"/>
+    </row>
+    <row r="78" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A78" s="24"/>
+      <c r="B78" s="24"/>
+      <c r="C78" s="24"/>
+      <c r="D78" s="24"/>
+      <c r="E78" s="24"/>
+      <c r="F78" s="24"/>
+      <c r="G78" s="24"/>
+      <c r="H78" s="24"/>
+      <c r="I78" s="24"/>
+      <c r="J78" s="24"/>
+      <c r="K78" s="24"/>
+      <c r="L78" s="24"/>
+      <c r="M78" s="24"/>
+    </row>
+    <row r="79" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A79" s="24"/>
+      <c r="B79" s="24"/>
+      <c r="C79" s="24"/>
+      <c r="D79" s="24"/>
+      <c r="E79" s="24"/>
+      <c r="F79" s="24"/>
+      <c r="G79" s="24"/>
+      <c r="H79" s="24"/>
+      <c r="I79" s="24"/>
+      <c r="J79" s="24"/>
+      <c r="K79" s="24"/>
+      <c r="L79" s="24"/>
+      <c r="M79" s="24"/>
+    </row>
+    <row r="80" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A80" s="24"/>
+      <c r="B80" s="24"/>
+      <c r="C80" s="24"/>
+      <c r="D80" s="24"/>
+      <c r="E80" s="24"/>
+      <c r="F80" s="24"/>
+      <c r="G80" s="24"/>
+      <c r="H80" s="24"/>
+      <c r="I80" s="24"/>
+      <c r="J80" s="24"/>
+      <c r="K80" s="24"/>
+      <c r="L80" s="24"/>
+      <c r="M80" s="24"/>
+    </row>
+    <row r="81" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A81" s="24"/>
+      <c r="B81" s="24"/>
+      <c r="C81" s="24"/>
+      <c r="D81" s="24"/>
+      <c r="E81" s="24"/>
+      <c r="F81" s="24"/>
+      <c r="G81" s="24"/>
+      <c r="H81" s="24"/>
+      <c r="I81" s="24"/>
+      <c r="J81" s="24"/>
+      <c r="K81" s="24"/>
+      <c r="L81" s="24"/>
+      <c r="M81" s="24"/>
+    </row>
+    <row r="82" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A82" s="24"/>
+      <c r="B82" s="24"/>
+      <c r="C82" s="24"/>
+      <c r="D82" s="24"/>
+      <c r="E82" s="24"/>
+      <c r="F82" s="24"/>
+      <c r="G82" s="24"/>
+      <c r="H82" s="24"/>
+      <c r="I82" s="24"/>
+      <c r="J82" s="24"/>
+      <c r="K82" s="24"/>
+      <c r="L82" s="24"/>
+      <c r="M82" s="24"/>
+    </row>
+    <row r="83" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A83" s="24"/>
+      <c r="B83" s="24"/>
+      <c r="C83" s="24"/>
+      <c r="D83" s="24"/>
+      <c r="E83" s="24"/>
+      <c r="F83" s="24"/>
+      <c r="G83" s="24"/>
+      <c r="H83" s="24"/>
+      <c r="I83" s="24"/>
+      <c r="J83" s="24"/>
+      <c r="K83" s="24"/>
+      <c r="L83" s="24"/>
+      <c r="M83" s="24"/>
+    </row>
+    <row r="84" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A84" s="24"/>
+      <c r="B84" s="24"/>
+      <c r="C84" s="24"/>
+      <c r="D84" s="24"/>
+      <c r="E84" s="24"/>
+      <c r="F84" s="24"/>
+      <c r="G84" s="24"/>
+      <c r="H84" s="24"/>
+      <c r="I84" s="24"/>
+      <c r="J84" s="24"/>
+      <c r="K84" s="24"/>
+      <c r="L84" s="24"/>
+      <c r="M84" s="24"/>
+    </row>
+    <row r="85" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A85" s="24"/>
+      <c r="B85" s="24"/>
+      <c r="C85" s="24"/>
+      <c r="D85" s="24"/>
+      <c r="E85" s="24"/>
+      <c r="F85" s="24"/>
+      <c r="G85" s="24"/>
+      <c r="H85" s="24"/>
+      <c r="I85" s="24"/>
+      <c r="J85" s="24"/>
+      <c r="K85" s="24"/>
+      <c r="L85" s="24"/>
+      <c r="M85" s="24"/>
+    </row>
+    <row r="86" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A86" s="24"/>
+      <c r="B86" s="24"/>
+      <c r="C86" s="24"/>
+      <c r="D86" s="24"/>
+      <c r="E86" s="24"/>
+      <c r="F86" s="24"/>
+      <c r="G86" s="24"/>
+      <c r="H86" s="24"/>
+      <c r="I86" s="24"/>
+      <c r="J86" s="24"/>
+      <c r="K86" s="24"/>
+      <c r="L86" s="24"/>
+      <c r="M86" s="24"/>
+    </row>
+    <row r="87" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A87" s="24"/>
+      <c r="B87" s="24"/>
+      <c r="C87" s="24"/>
+      <c r="D87" s="24"/>
+      <c r="E87" s="24"/>
+      <c r="F87" s="24"/>
+      <c r="G87" s="24"/>
+      <c r="H87" s="24"/>
+      <c r="I87" s="24"/>
+      <c r="J87" s="24"/>
+      <c r="K87" s="24"/>
+      <c r="L87" s="24"/>
+      <c r="M87" s="24"/>
+    </row>
+    <row r="88" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A88" s="24"/>
+      <c r="B88" s="24"/>
+      <c r="C88" s="24"/>
+      <c r="D88" s="24"/>
+      <c r="E88" s="24"/>
+      <c r="F88" s="24"/>
+      <c r="G88" s="24"/>
+      <c r="H88" s="24"/>
+      <c r="I88" s="24"/>
+      <c r="J88" s="24"/>
+      <c r="K88" s="24"/>
+      <c r="L88" s="24"/>
+      <c r="M88" s="24"/>
+    </row>
+    <row r="89" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A89" s="24"/>
+      <c r="B89" s="24"/>
+      <c r="C89" s="24"/>
+      <c r="D89" s="24"/>
+      <c r="E89" s="24"/>
+      <c r="F89" s="24"/>
+      <c r="G89" s="24"/>
+      <c r="H89" s="24"/>
+      <c r="I89" s="24"/>
+      <c r="J89" s="24"/>
+      <c r="K89" s="24"/>
+      <c r="L89" s="24"/>
+      <c r="M89" s="24"/>
+    </row>
+    <row r="90" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A90" s="24"/>
+      <c r="B90" s="24"/>
+      <c r="C90" s="24"/>
+      <c r="D90" s="24"/>
+      <c r="E90" s="24"/>
+      <c r="F90" s="24"/>
+      <c r="G90" s="24"/>
+      <c r="H90" s="24"/>
+      <c r="I90" s="24"/>
+      <c r="J90" s="24"/>
+      <c r="K90" s="24"/>
+      <c r="L90" s="24"/>
+      <c r="M90" s="24"/>
+    </row>
+    <row r="91" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A91" s="24"/>
+      <c r="B91" s="24"/>
+      <c r="C91" s="24"/>
+      <c r="D91" s="24"/>
+      <c r="E91" s="24"/>
+      <c r="F91" s="24"/>
+      <c r="G91" s="24"/>
+      <c r="H91" s="24"/>
+      <c r="I91" s="24"/>
+      <c r="J91" s="24"/>
+      <c r="K91" s="24"/>
+      <c r="L91" s="24"/>
+      <c r="M91" s="24"/>
+    </row>
+    <row r="92" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A92" s="24"/>
+      <c r="B92" s="24"/>
+      <c r="C92" s="24"/>
+      <c r="D92" s="24"/>
+      <c r="E92" s="24"/>
+      <c r="F92" s="24"/>
+      <c r="G92" s="24"/>
+      <c r="H92" s="24"/>
+      <c r="I92" s="24"/>
+      <c r="J92" s="24"/>
+      <c r="K92" s="24"/>
+      <c r="L92" s="24"/>
+      <c r="M92" s="24"/>
+    </row>
+    <row r="93" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A93" s="24"/>
+      <c r="B93" s="24"/>
+      <c r="C93" s="24"/>
+      <c r="D93" s="24"/>
+      <c r="E93" s="24"/>
+      <c r="F93" s="24"/>
+      <c r="G93" s="24"/>
+      <c r="H93" s="24"/>
+      <c r="I93" s="24"/>
+      <c r="J93" s="24"/>
+      <c r="K93" s="24"/>
+      <c r="L93" s="24"/>
+      <c r="M93" s="24"/>
+    </row>
+    <row r="94" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A94" s="24"/>
+      <c r="B94" s="24"/>
+      <c r="C94" s="24"/>
+      <c r="D94" s="24"/>
+      <c r="E94" s="24"/>
+      <c r="F94" s="24"/>
+      <c r="G94" s="24"/>
+      <c r="H94" s="24"/>
+      <c r="I94" s="24"/>
+      <c r="J94" s="24"/>
+      <c r="K94" s="24"/>
+      <c r="L94" s="24"/>
+      <c r="M94" s="24"/>
+    </row>
+    <row r="95" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A95" s="24"/>
+      <c r="B95" s="24"/>
+      <c r="C95" s="24"/>
+      <c r="D95" s="24"/>
+      <c r="E95" s="24"/>
+      <c r="F95" s="24"/>
+      <c r="G95" s="24"/>
+      <c r="H95" s="24"/>
+      <c r="I95" s="24"/>
+      <c r="J95" s="24"/>
+      <c r="K95" s="24"/>
+      <c r="L95" s="24"/>
+      <c r="M95" s="24"/>
+    </row>
+    <row r="96" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A96" s="24"/>
+      <c r="B96" s="24"/>
+      <c r="C96" s="24"/>
+      <c r="D96" s="24"/>
+      <c r="E96" s="24"/>
+      <c r="F96" s="24"/>
+      <c r="G96" s="24"/>
+      <c r="H96" s="24"/>
+      <c r="I96" s="24"/>
+      <c r="J96" s="24"/>
+      <c r="K96" s="24"/>
+      <c r="L96" s="24"/>
+      <c r="M96" s="24"/>
+    </row>
+    <row r="97" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A97" s="24"/>
+      <c r="B97" s="24"/>
+      <c r="C97" s="24"/>
+      <c r="D97" s="24"/>
+      <c r="E97" s="24"/>
+      <c r="F97" s="24"/>
+      <c r="G97" s="24"/>
+      <c r="H97" s="24"/>
+      <c r="I97" s="24"/>
+      <c r="J97" s="24"/>
+      <c r="K97" s="24"/>
+      <c r="L97" s="24"/>
+      <c r="M97" s="24"/>
+    </row>
+    <row r="98" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A98" s="24"/>
+      <c r="B98" s="24"/>
+      <c r="C98" s="24"/>
+      <c r="D98" s="24"/>
+      <c r="E98" s="24"/>
+      <c r="F98" s="24"/>
+      <c r="G98" s="24"/>
+      <c r="H98" s="24"/>
+      <c r="I98" s="24"/>
+      <c r="J98" s="24"/>
+      <c r="K98" s="24"/>
+      <c r="L98" s="24"/>
+      <c r="M98" s="24"/>
+    </row>
+    <row r="99" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A99" s="24"/>
+      <c r="B99" s="24"/>
+      <c r="C99" s="24"/>
+      <c r="D99" s="24"/>
+      <c r="E99" s="24"/>
+      <c r="F99" s="24"/>
+      <c r="G99" s="24"/>
+      <c r="H99" s="24"/>
+      <c r="I99" s="24"/>
+      <c r="J99" s="24"/>
+      <c r="K99" s="24"/>
+      <c r="L99" s="24"/>
+      <c r="M99" s="24"/>
+    </row>
+    <row r="100" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A100" s="24"/>
+      <c r="B100" s="24"/>
+      <c r="C100" s="24"/>
+      <c r="D100" s="24"/>
+      <c r="E100" s="24"/>
+      <c r="F100" s="24"/>
+      <c r="G100" s="24"/>
+      <c r="H100" s="24"/>
+      <c r="I100" s="24"/>
+      <c r="J100" s="24"/>
+      <c r="K100" s="24"/>
+      <c r="L100" s="24"/>
+      <c r="M100" s="24"/>
+    </row>
+    <row r="101" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A101" s="24"/>
+      <c r="B101" s="24"/>
+      <c r="C101" s="24"/>
+      <c r="D101" s="24"/>
+      <c r="E101" s="24"/>
+      <c r="F101" s="24"/>
+      <c r="G101" s="24"/>
+      <c r="H101" s="24"/>
+      <c r="I101" s="24"/>
+      <c r="J101" s="24"/>
+      <c r="K101" s="24"/>
+      <c r="L101" s="24"/>
+      <c r="M101" s="24"/>
+    </row>
+    <row r="102" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A102" s="24"/>
+      <c r="B102" s="24"/>
+      <c r="C102" s="24"/>
+      <c r="D102" s="24"/>
+      <c r="E102" s="24"/>
+      <c r="F102" s="24"/>
+      <c r="G102" s="24"/>
+      <c r="H102" s="24"/>
+      <c r="I102" s="24"/>
+      <c r="J102" s="24"/>
+      <c r="K102" s="24"/>
+      <c r="L102" s="24"/>
+      <c r="M102" s="24"/>
+    </row>
+    <row r="103" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A103" s="24"/>
+      <c r="B103" s="24"/>
+      <c r="C103" s="24"/>
+      <c r="D103" s="24"/>
+      <c r="E103" s="24"/>
+      <c r="F103" s="24"/>
+      <c r="G103" s="24"/>
+      <c r="H103" s="24"/>
+      <c r="I103" s="24"/>
+      <c r="J103" s="24"/>
+      <c r="K103" s="24"/>
+      <c r="L103" s="24"/>
+      <c r="M103" s="24"/>
+    </row>
+    <row r="104" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A104" s="24"/>
+      <c r="B104" s="24"/>
+      <c r="C104" s="24"/>
+      <c r="D104" s="24"/>
+      <c r="E104" s="24"/>
+      <c r="F104" s="24"/>
+      <c r="G104" s="24"/>
+      <c r="H104" s="24"/>
+      <c r="I104" s="24"/>
+      <c r="J104" s="24"/>
+      <c r="K104" s="24"/>
+      <c r="L104" s="24"/>
+      <c r="M104" s="24"/>
+    </row>
+    <row r="105" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A105" s="24"/>
+      <c r="B105" s="24"/>
+      <c r="C105" s="24"/>
+      <c r="D105" s="24"/>
+      <c r="E105" s="24"/>
+      <c r="F105" s="24"/>
+      <c r="G105" s="24"/>
+      <c r="H105" s="24"/>
+      <c r="I105" s="24"/>
+      <c r="J105" s="24"/>
+      <c r="K105" s="24"/>
+      <c r="L105" s="24"/>
+      <c r="M105" s="24"/>
+    </row>
+    <row r="106" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A106" s="24"/>
+      <c r="B106" s="24"/>
+      <c r="C106" s="24"/>
+      <c r="D106" s="24"/>
+      <c r="E106" s="24"/>
+      <c r="F106" s="24"/>
+      <c r="G106" s="24"/>
+      <c r="H106" s="24"/>
+      <c r="I106" s="24"/>
+      <c r="J106" s="24"/>
+      <c r="K106" s="24"/>
+      <c r="L106" s="24"/>
+      <c r="M106" s="24"/>
+    </row>
+    <row r="107" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A107" s="24"/>
+      <c r="B107" s="24"/>
+      <c r="C107" s="24"/>
+      <c r="D107" s="24"/>
+      <c r="E107" s="24"/>
+      <c r="F107" s="24"/>
+      <c r="G107" s="24"/>
+      <c r="H107" s="24"/>
+      <c r="I107" s="24"/>
+      <c r="J107" s="24"/>
+      <c r="K107" s="24"/>
+      <c r="L107" s="24"/>
+      <c r="M107" s="24"/>
+    </row>
+    <row r="108" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A108" s="24"/>
+      <c r="B108" s="24"/>
+      <c r="C108" s="24"/>
+      <c r="D108" s="24"/>
+      <c r="E108" s="24"/>
+      <c r="F108" s="24"/>
+      <c r="G108" s="24"/>
+      <c r="H108" s="24"/>
+      <c r="I108" s="24"/>
+      <c r="J108" s="24"/>
+      <c r="K108" s="24"/>
+      <c r="L108" s="24"/>
+      <c r="M108" s="24"/>
+    </row>
+    <row r="109" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A109" s="24"/>
+      <c r="B109" s="24"/>
+      <c r="C109" s="24"/>
+      <c r="D109" s="24"/>
+      <c r="E109" s="24"/>
+      <c r="F109" s="24"/>
+      <c r="G109" s="24"/>
+      <c r="H109" s="24"/>
+      <c r="I109" s="24"/>
+      <c r="J109" s="24"/>
+      <c r="K109" s="24"/>
+      <c r="L109" s="24"/>
+      <c r="M109" s="24"/>
+    </row>
+    <row r="110" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A110" s="24"/>
+      <c r="B110" s="24"/>
+      <c r="C110" s="24"/>
+      <c r="D110" s="24"/>
+      <c r="E110" s="24"/>
+      <c r="F110" s="24"/>
+      <c r="G110" s="24"/>
+      <c r="H110" s="24"/>
+      <c r="I110" s="24"/>
+      <c r="J110" s="24"/>
+      <c r="K110" s="24"/>
+      <c r="L110" s="24"/>
+      <c r="M110" s="24"/>
+    </row>
+    <row r="111" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A111" s="24"/>
+      <c r="B111" s="24"/>
+      <c r="C111" s="24"/>
+      <c r="D111" s="24"/>
+      <c r="E111" s="24"/>
+      <c r="F111" s="24"/>
+      <c r="G111" s="24"/>
+      <c r="H111" s="24"/>
+      <c r="I111" s="24"/>
+      <c r="J111" s="24"/>
+      <c r="K111" s="24"/>
+      <c r="L111" s="24"/>
+      <c r="M111" s="24"/>
+    </row>
+    <row r="112" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A112" s="24"/>
+      <c r="B112" s="24"/>
+      <c r="C112" s="24"/>
+      <c r="D112" s="24"/>
+      <c r="E112" s="24"/>
+      <c r="F112" s="24"/>
+      <c r="G112" s="24"/>
+      <c r="H112" s="24"/>
+      <c r="I112" s="24"/>
+      <c r="J112" s="24"/>
+      <c r="K112" s="24"/>
+      <c r="L112" s="24"/>
+      <c r="M112" s="24"/>
+    </row>
+    <row r="113" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A113" s="24"/>
+      <c r="B113" s="24"/>
+      <c r="C113" s="24"/>
+      <c r="D113" s="24"/>
+      <c r="E113" s="24"/>
+      <c r="F113" s="24"/>
+      <c r="G113" s="24"/>
+      <c r="H113" s="24"/>
+      <c r="I113" s="24"/>
+      <c r="J113" s="24"/>
+      <c r="K113" s="24"/>
+      <c r="L113" s="24"/>
+      <c r="M113" s="24"/>
+    </row>
+    <row r="114" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A114" s="24"/>
+      <c r="B114" s="24"/>
+      <c r="C114" s="24"/>
+      <c r="D114" s="24"/>
+      <c r="E114" s="24"/>
+      <c r="F114" s="24"/>
+      <c r="G114" s="24"/>
+      <c r="H114" s="24"/>
+      <c r="I114" s="24"/>
+      <c r="J114" s="24"/>
+      <c r="K114" s="24"/>
+      <c r="L114" s="24"/>
+      <c r="M114" s="24"/>
+    </row>
+    <row r="115" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A115" s="24"/>
+      <c r="B115" s="24"/>
+      <c r="C115" s="24"/>
+      <c r="D115" s="24"/>
+      <c r="E115" s="24"/>
+      <c r="F115" s="24"/>
+      <c r="G115" s="24"/>
+      <c r="H115" s="24"/>
+      <c r="I115" s="24"/>
+      <c r="J115" s="24"/>
+      <c r="K115" s="24"/>
+      <c r="L115" s="24"/>
+      <c r="M115" s="24"/>
+    </row>
+    <row r="116" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A116" s="24"/>
+      <c r="B116" s="24"/>
+      <c r="C116" s="24"/>
+      <c r="D116" s="24"/>
+      <c r="E116" s="24"/>
+      <c r="F116" s="24"/>
+      <c r="G116" s="24"/>
+      <c r="H116" s="24"/>
+      <c r="I116" s="24"/>
+      <c r="J116" s="24"/>
+      <c r="K116" s="24"/>
+      <c r="L116" s="24"/>
+      <c r="M116" s="24"/>
+    </row>
+    <row r="117" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A117" s="24"/>
+      <c r="B117" s="24"/>
+      <c r="C117" s="24"/>
+      <c r="D117" s="24"/>
+      <c r="E117" s="24"/>
+      <c r="F117" s="24"/>
+      <c r="G117" s="24"/>
+      <c r="H117" s="24"/>
+      <c r="I117" s="24"/>
+      <c r="J117" s="24"/>
+      <c r="K117" s="24"/>
+      <c r="L117" s="24"/>
+      <c r="M117" s="24"/>
+    </row>
+    <row r="118" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A118" s="24"/>
+      <c r="B118" s="24"/>
+      <c r="C118" s="24"/>
+      <c r="D118" s="24"/>
+      <c r="E118" s="24"/>
+      <c r="F118" s="24"/>
+      <c r="G118" s="24"/>
+      <c r="H118" s="24"/>
+      <c r="I118" s="24"/>
+      <c r="J118" s="24"/>
+      <c r="K118" s="24"/>
+      <c r="L118" s="24"/>
+      <c r="M118" s="24"/>
+    </row>
+    <row r="119" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A119" s="24"/>
+      <c r="B119" s="24"/>
+      <c r="C119" s="24"/>
+      <c r="D119" s="24"/>
+      <c r="E119" s="24"/>
+      <c r="F119" s="24"/>
+      <c r="G119" s="24"/>
+      <c r="H119" s="24"/>
+      <c r="I119" s="24"/>
+      <c r="J119" s="24"/>
+      <c r="K119" s="24"/>
+      <c r="L119" s="24"/>
+      <c r="M119" s="24"/>
+    </row>
+    <row r="120" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A120" s="24"/>
+      <c r="B120" s="24"/>
+      <c r="C120" s="24"/>
+      <c r="D120" s="24"/>
+      <c r="E120" s="24"/>
+      <c r="F120" s="24"/>
+      <c r="G120" s="24"/>
+      <c r="H120" s="24"/>
+      <c r="I120" s="24"/>
+      <c r="J120" s="24"/>
+      <c r="K120" s="24"/>
+      <c r="L120" s="24"/>
+      <c r="M120" s="24"/>
+    </row>
+    <row r="121" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A121" s="24"/>
+      <c r="B121" s="24"/>
+      <c r="C121" s="24"/>
+      <c r="D121" s="24"/>
+      <c r="E121" s="24"/>
+      <c r="F121" s="24"/>
+      <c r="G121" s="24"/>
+      <c r="H121" s="24"/>
+      <c r="I121" s="24"/>
+      <c r="J121" s="24"/>
+      <c r="K121" s="24"/>
+      <c r="L121" s="24"/>
+      <c r="M121" s="24"/>
+    </row>
+    <row r="122" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A122" s="24"/>
+      <c r="B122" s="24"/>
+      <c r="C122" s="24"/>
+      <c r="D122" s="24"/>
+      <c r="E122" s="24"/>
+      <c r="F122" s="24"/>
+      <c r="G122" s="24"/>
+      <c r="H122" s="24"/>
+      <c r="I122" s="24"/>
+      <c r="J122" s="24"/>
+      <c r="K122" s="24"/>
+      <c r="L122" s="24"/>
+      <c r="M122" s="24"/>
+    </row>
+    <row r="123" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A123" s="24"/>
+      <c r="B123" s="24"/>
+      <c r="C123" s="24"/>
+      <c r="D123" s="24"/>
+      <c r="E123" s="24"/>
+      <c r="F123" s="24"/>
+      <c r="G123" s="24"/>
+      <c r="H123" s="24"/>
+      <c r="I123" s="24"/>
+      <c r="J123" s="24"/>
+      <c r="K123" s="24"/>
+      <c r="L123" s="24"/>
+      <c r="M123" s="24"/>
+    </row>
+    <row r="124" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A124" s="24"/>
+      <c r="B124" s="24"/>
+      <c r="C124" s="24"/>
+      <c r="D124" s="24"/>
+      <c r="E124" s="24"/>
+      <c r="F124" s="24"/>
+      <c r="G124" s="24"/>
+      <c r="H124" s="24"/>
+      <c r="I124" s="24"/>
+      <c r="J124" s="24"/>
+      <c r="K124" s="24"/>
+      <c r="L124" s="24"/>
+      <c r="M124" s="24"/>
+    </row>
+    <row r="125" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A125" s="24"/>
+      <c r="B125" s="24"/>
+      <c r="C125" s="24"/>
+      <c r="D125" s="24"/>
+      <c r="E125" s="24"/>
+      <c r="F125" s="24"/>
+      <c r="G125" s="24"/>
+      <c r="H125" s="24"/>
+      <c r="I125" s="24"/>
+      <c r="J125" s="24"/>
+      <c r="K125" s="24"/>
+      <c r="L125" s="24"/>
+      <c r="M125" s="24"/>
+    </row>
+    <row r="126" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A126" s="24"/>
+      <c r="B126" s="24"/>
+      <c r="C126" s="24"/>
+      <c r="D126" s="24"/>
+      <c r="E126" s="24"/>
+      <c r="F126" s="24"/>
+      <c r="G126" s="24"/>
+      <c r="H126" s="24"/>
+      <c r="I126" s="24"/>
+      <c r="J126" s="24"/>
+      <c r="K126" s="24"/>
+      <c r="L126" s="24"/>
+      <c r="M126" s="24"/>
+    </row>
+    <row r="127" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A127" s="24"/>
+      <c r="B127" s="24"/>
+      <c r="C127" s="24"/>
+      <c r="D127" s="24"/>
+      <c r="E127" s="24"/>
+      <c r="F127" s="24"/>
+      <c r="G127" s="24"/>
+      <c r="H127" s="24"/>
+      <c r="I127" s="24"/>
+      <c r="J127" s="24"/>
+      <c r="K127" s="24"/>
+      <c r="L127" s="24"/>
+      <c r="M127" s="24"/>
+    </row>
+    <row r="128" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A128" s="24"/>
+      <c r="B128" s="24"/>
+      <c r="C128" s="24"/>
+      <c r="D128" s="24"/>
+      <c r="E128" s="24"/>
+      <c r="F128" s="24"/>
+      <c r="G128" s="24"/>
+      <c r="H128" s="24"/>
+      <c r="I128" s="24"/>
+      <c r="J128" s="24"/>
+      <c r="K128" s="24"/>
+      <c r="L128" s="24"/>
+      <c r="M128" s="24"/>
+    </row>
+    <row r="129" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A129" s="24"/>
+      <c r="B129" s="24"/>
+      <c r="C129" s="24"/>
+      <c r="D129" s="24"/>
+      <c r="E129" s="24"/>
+      <c r="F129" s="24"/>
+      <c r="G129" s="24"/>
+      <c r="H129" s="24"/>
+      <c r="I129" s="24"/>
+      <c r="J129" s="24"/>
+      <c r="K129" s="24"/>
+      <c r="L129" s="24"/>
+      <c r="M129" s="24"/>
+    </row>
+    <row r="130" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A130" s="24"/>
+      <c r="B130" s="24"/>
+      <c r="C130" s="24"/>
+      <c r="D130" s="24"/>
+      <c r="E130" s="24"/>
+      <c r="F130" s="24"/>
+      <c r="G130" s="24"/>
+      <c r="H130" s="24"/>
+      <c r="I130" s="24"/>
+      <c r="J130" s="24"/>
+      <c r="K130" s="24"/>
+      <c r="L130" s="24"/>
+      <c r="M130" s="24"/>
+    </row>
+    <row r="131" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A131" s="24"/>
+      <c r="B131" s="24"/>
+      <c r="C131" s="24"/>
+      <c r="D131" s="24"/>
+      <c r="E131" s="24"/>
+      <c r="F131" s="24"/>
+      <c r="G131" s="24"/>
+      <c r="H131" s="24"/>
+      <c r="I131" s="24"/>
+      <c r="J131" s="24"/>
+      <c r="K131" s="24"/>
+      <c r="L131" s="24"/>
+      <c r="M131" s="24"/>
+    </row>
+    <row r="132" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A132" s="24"/>
+      <c r="B132" s="24"/>
+      <c r="C132" s="24"/>
+      <c r="D132" s="24"/>
+      <c r="E132" s="24"/>
+      <c r="F132" s="24"/>
+      <c r="G132" s="24"/>
+      <c r="H132" s="24"/>
+      <c r="I132" s="24"/>
+      <c r="J132" s="24"/>
+      <c r="K132" s="24"/>
+      <c r="L132" s="24"/>
+      <c r="M132" s="24"/>
+    </row>
+    <row r="133" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A133" s="24"/>
+      <c r="B133" s="24"/>
+      <c r="C133" s="24"/>
+      <c r="D133" s="24"/>
+      <c r="E133" s="24"/>
+      <c r="F133" s="24"/>
+      <c r="G133" s="24"/>
+      <c r="H133" s="24"/>
+      <c r="I133" s="24"/>
+      <c r="J133" s="24"/>
+      <c r="K133" s="24"/>
+      <c r="L133" s="24"/>
+      <c r="M133" s="24"/>
+    </row>
+    <row r="134" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A134" s="24"/>
+      <c r="B134" s="24"/>
+      <c r="C134" s="24"/>
+      <c r="D134" s="24"/>
+      <c r="E134" s="24"/>
+      <c r="F134" s="24"/>
+      <c r="G134" s="24"/>
+      <c r="H134" s="24"/>
+      <c r="I134" s="24"/>
+      <c r="J134" s="24"/>
+      <c r="K134" s="24"/>
+      <c r="L134" s="24"/>
+      <c r="M134" s="24"/>
+    </row>
+    <row r="135" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A135" s="24"/>
+      <c r="B135" s="24"/>
+      <c r="C135" s="24"/>
+      <c r="D135" s="24"/>
+      <c r="E135" s="24"/>
+      <c r="F135" s="24"/>
+      <c r="G135" s="24"/>
+      <c r="H135" s="24"/>
+      <c r="I135" s="24"/>
+      <c r="J135" s="24"/>
+      <c r="K135" s="24"/>
+      <c r="L135" s="24"/>
+      <c r="M135" s="24"/>
+    </row>
+    <row r="136" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A136" s="24"/>
+      <c r="B136" s="24"/>
+      <c r="C136" s="24"/>
+      <c r="D136" s="24"/>
+      <c r="E136" s="24"/>
+      <c r="F136" s="24"/>
+      <c r="G136" s="24"/>
+      <c r="H136" s="24"/>
+      <c r="I136" s="24"/>
+      <c r="J136" s="24"/>
+      <c r="K136" s="24"/>
+      <c r="L136" s="24"/>
+      <c r="M136" s="24"/>
+    </row>
+    <row r="137" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A137" s="24"/>
+      <c r="B137" s="24"/>
+      <c r="C137" s="24"/>
+      <c r="D137" s="24"/>
+      <c r="E137" s="24"/>
+      <c r="F137" s="24"/>
+      <c r="G137" s="24"/>
+      <c r="H137" s="24"/>
+      <c r="I137" s="24"/>
+      <c r="J137" s="24"/>
+      <c r="K137" s="24"/>
+      <c r="L137" s="24"/>
+      <c r="M137" s="24"/>
+    </row>
+    <row r="138" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A138" s="24"/>
+      <c r="B138" s="24"/>
+      <c r="C138" s="24"/>
+      <c r="D138" s="24"/>
+      <c r="E138" s="24"/>
+      <c r="F138" s="24"/>
+      <c r="G138" s="24"/>
+      <c r="H138" s="24"/>
+      <c r="I138" s="24"/>
+      <c r="J138" s="24"/>
+      <c r="K138" s="24"/>
+      <c r="L138" s="24"/>
+      <c r="M138" s="24"/>
+    </row>
+    <row r="139" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A139" s="24"/>
+      <c r="B139" s="24"/>
+      <c r="C139" s="24"/>
+      <c r="D139" s="24"/>
+      <c r="E139" s="24"/>
+      <c r="F139" s="24"/>
+      <c r="G139" s="24"/>
+      <c r="H139" s="24"/>
+      <c r="I139" s="24"/>
+      <c r="J139" s="24"/>
+      <c r="K139" s="24"/>
+      <c r="L139" s="24"/>
+      <c r="M139" s="24"/>
+    </row>
+    <row r="140" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A140" s="24"/>
+      <c r="B140" s="24"/>
+      <c r="C140" s="24"/>
+      <c r="D140" s="24"/>
+      <c r="E140" s="24"/>
+      <c r="F140" s="24"/>
+      <c r="G140" s="24"/>
+      <c r="H140" s="24"/>
+      <c r="I140" s="24"/>
+      <c r="J140" s="24"/>
+      <c r="K140" s="24"/>
+      <c r="L140" s="24"/>
+      <c r="M140" s="24"/>
+    </row>
+    <row r="141" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A141" s="24"/>
+      <c r="B141" s="24"/>
+      <c r="C141" s="24"/>
+      <c r="D141" s="24"/>
+      <c r="E141" s="24"/>
+      <c r="F141" s="24"/>
+      <c r="G141" s="24"/>
+      <c r="H141" s="24"/>
+      <c r="I141" s="24"/>
+      <c r="J141" s="24"/>
+      <c r="K141" s="24"/>
+      <c r="L141" s="24"/>
+      <c r="M141" s="24"/>
+    </row>
+    <row r="142" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A142" s="24"/>
+      <c r="B142" s="24"/>
+      <c r="C142" s="24"/>
+      <c r="D142" s="24"/>
+      <c r="E142" s="24"/>
+      <c r="F142" s="24"/>
+      <c r="G142" s="24"/>
+      <c r="H142" s="24"/>
+      <c r="I142" s="24"/>
+      <c r="J142" s="24"/>
+      <c r="K142" s="24"/>
+      <c r="L142" s="24"/>
+      <c r="M142" s="24"/>
+    </row>
+    <row r="143" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A143" s="24"/>
+      <c r="B143" s="24"/>
+      <c r="C143" s="24"/>
+      <c r="D143" s="24"/>
+      <c r="E143" s="24"/>
+      <c r="F143" s="24"/>
+      <c r="G143" s="24"/>
+      <c r="H143" s="24"/>
+      <c r="I143" s="24"/>
+      <c r="J143" s="24"/>
+      <c r="K143" s="24"/>
+      <c r="L143" s="24"/>
+      <c r="M143" s="24"/>
+    </row>
+    <row r="144" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A144" s="24"/>
+      <c r="B144" s="24"/>
+      <c r="C144" s="24"/>
+      <c r="D144" s="24"/>
+      <c r="E144" s="24"/>
+      <c r="F144" s="24"/>
+      <c r="G144" s="24"/>
+      <c r="H144" s="24"/>
+      <c r="I144" s="24"/>
+      <c r="J144" s="24"/>
+      <c r="K144" s="24"/>
+      <c r="L144" s="24"/>
+      <c r="M144" s="24"/>
+    </row>
+    <row r="145" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A145" s="24"/>
+      <c r="B145" s="24"/>
+      <c r="C145" s="24"/>
+      <c r="D145" s="24"/>
+      <c r="E145" s="24"/>
+      <c r="F145" s="24"/>
+      <c r="G145" s="24"/>
+      <c r="H145" s="24"/>
+      <c r="I145" s="24"/>
+      <c r="J145" s="24"/>
+      <c r="K145" s="24"/>
+      <c r="L145" s="24"/>
+      <c r="M145" s="24"/>
+    </row>
+    <row r="146" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A146" s="24"/>
+      <c r="B146" s="24"/>
+      <c r="C146" s="24"/>
+      <c r="D146" s="24"/>
+      <c r="E146" s="24"/>
+      <c r="F146" s="24"/>
+      <c r="G146" s="24"/>
+      <c r="H146" s="24"/>
+      <c r="I146" s="24"/>
+      <c r="J146" s="24"/>
+      <c r="K146" s="24"/>
+      <c r="L146" s="24"/>
+      <c r="M146" s="24"/>
+    </row>
+    <row r="147" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A147" s="24"/>
+      <c r="B147" s="24"/>
+      <c r="C147" s="24"/>
+      <c r="D147" s="24"/>
+      <c r="E147" s="24"/>
+      <c r="F147" s="24"/>
+      <c r="G147" s="24"/>
+      <c r="H147" s="24"/>
+      <c r="I147" s="24"/>
+      <c r="J147" s="24"/>
+      <c r="K147" s="24"/>
+      <c r="L147" s="24"/>
+      <c r="M147" s="24"/>
+    </row>
+    <row r="148" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A148" s="24"/>
+      <c r="B148" s="24"/>
+      <c r="C148" s="24"/>
+      <c r="D148" s="24"/>
+      <c r="E148" s="24"/>
+      <c r="F148" s="24"/>
+      <c r="G148" s="24"/>
+      <c r="H148" s="24"/>
+      <c r="I148" s="24"/>
+      <c r="J148" s="24"/>
+      <c r="K148" s="24"/>
+      <c r="L148" s="24"/>
+      <c r="M148" s="24"/>
+    </row>
+    <row r="149" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A149" s="24"/>
+      <c r="B149" s="24"/>
+      <c r="C149" s="24"/>
+      <c r="D149" s="24"/>
+      <c r="E149" s="24"/>
+      <c r="F149" s="24"/>
+      <c r="G149" s="24"/>
+      <c r="H149" s="24"/>
+      <c r="I149" s="24"/>
+      <c r="J149" s="24"/>
+      <c r="K149" s="24"/>
+      <c r="L149" s="24"/>
+      <c r="M149" s="24"/>
+    </row>
+    <row r="150" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A150" s="24"/>
+      <c r="B150" s="24"/>
+      <c r="C150" s="24"/>
+      <c r="D150" s="24"/>
+      <c r="E150" s="24"/>
+      <c r="F150" s="24"/>
+      <c r="G150" s="24"/>
+      <c r="H150" s="24"/>
+      <c r="I150" s="24"/>
+      <c r="J150" s="24"/>
+      <c r="K150" s="24"/>
+      <c r="L150" s="24"/>
+      <c r="M150" s="24"/>
+    </row>
+    <row r="151" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A151" s="24"/>
+      <c r="B151" s="24"/>
+      <c r="C151" s="24"/>
+      <c r="D151" s="24"/>
+      <c r="E151" s="24"/>
+      <c r="F151" s="24"/>
+      <c r="G151" s="24"/>
+      <c r="H151" s="24"/>
+      <c r="I151" s="24"/>
+      <c r="J151" s="24"/>
+      <c r="K151" s="24"/>
+      <c r="L151" s="24"/>
+      <c r="M151" s="24"/>
+    </row>
+    <row r="152" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A152" s="24"/>
+      <c r="B152" s="24"/>
+      <c r="C152" s="24"/>
+      <c r="D152" s="24"/>
+      <c r="E152" s="24"/>
+      <c r="F152" s="24"/>
+      <c r="G152" s="24"/>
+      <c r="H152" s="24"/>
+      <c r="I152" s="24"/>
+      <c r="J152" s="24"/>
+      <c r="K152" s="24"/>
+      <c r="L152" s="24"/>
+      <c r="M152" s="24"/>
+    </row>
+    <row r="153" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A153" s="24"/>
+      <c r="B153" s="24"/>
+      <c r="C153" s="24"/>
+      <c r="D153" s="24"/>
+      <c r="E153" s="24"/>
+      <c r="F153" s="24"/>
+      <c r="G153" s="24"/>
+      <c r="H153" s="24"/>
+      <c r="I153" s="24"/>
+      <c r="J153" s="24"/>
+      <c r="K153" s="24"/>
+      <c r="L153" s="24"/>
+      <c r="M153" s="24"/>
+    </row>
+    <row r="154" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A154" s="24"/>
+      <c r="B154" s="24"/>
+      <c r="C154" s="24"/>
+      <c r="D154" s="24"/>
+      <c r="E154" s="24"/>
+      <c r="F154" s="24"/>
+      <c r="G154" s="24"/>
+      <c r="H154" s="24"/>
+      <c r="I154" s="24"/>
+      <c r="J154" s="24"/>
+      <c r="K154" s="24"/>
+      <c r="L154" s="24"/>
+      <c r="M154" s="24"/>
+    </row>
+    <row r="155" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A155" s="24"/>
+      <c r="B155" s="24"/>
+      <c r="C155" s="24"/>
+      <c r="D155" s="24"/>
+      <c r="E155" s="24"/>
+      <c r="F155" s="24"/>
+      <c r="G155" s="24"/>
+      <c r="H155" s="24"/>
+      <c r="I155" s="24"/>
+      <c r="J155" s="24"/>
+      <c r="K155" s="24"/>
+      <c r="L155" s="24"/>
+      <c r="M155" s="24"/>
+    </row>
+    <row r="156" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A156" s="24"/>
+      <c r="B156" s="24"/>
+      <c r="C156" s="24"/>
+      <c r="D156" s="24"/>
+      <c r="E156" s="24"/>
+      <c r="F156" s="24"/>
+      <c r="G156" s="24"/>
+      <c r="H156" s="24"/>
+      <c r="I156" s="24"/>
+      <c r="J156" s="24"/>
+      <c r="K156" s="24"/>
+      <c r="L156" s="24"/>
+      <c r="M156" s="24"/>
+    </row>
+    <row r="157" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A157" s="24"/>
+      <c r="B157" s="24"/>
+      <c r="C157" s="24"/>
+      <c r="D157" s="24"/>
+      <c r="E157" s="24"/>
+      <c r="F157" s="24"/>
+      <c r="G157" s="24"/>
+      <c r="H157" s="24"/>
+      <c r="I157" s="24"/>
+      <c r="J157" s="24"/>
+      <c r="K157" s="24"/>
+      <c r="L157" s="24"/>
+      <c r="M157" s="24"/>
+    </row>
+    <row r="158" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A158" s="24"/>
+      <c r="B158" s="24"/>
+      <c r="C158" s="24"/>
+      <c r="D158" s="24"/>
+      <c r="E158" s="24"/>
+      <c r="F158" s="24"/>
+      <c r="G158" s="24"/>
+      <c r="H158" s="24"/>
+      <c r="I158" s="24"/>
+      <c r="J158" s="24"/>
+      <c r="K158" s="24"/>
+      <c r="L158" s="24"/>
+      <c r="M158" s="24"/>
+    </row>
+    <row r="159" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A159" s="24"/>
+      <c r="B159" s="24"/>
+      <c r="C159" s="24"/>
+      <c r="D159" s="24"/>
+      <c r="E159" s="24"/>
+      <c r="F159" s="24"/>
+      <c r="G159" s="24"/>
+      <c r="H159" s="24"/>
+      <c r="I159" s="24"/>
+      <c r="J159" s="24"/>
+      <c r="K159" s="24"/>
+      <c r="L159" s="24"/>
+      <c r="M159" s="24"/>
+    </row>
+    <row r="160" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A160" s="24"/>
+      <c r="B160" s="24"/>
+      <c r="C160" s="24"/>
+      <c r="D160" s="24"/>
+      <c r="E160" s="24"/>
+      <c r="F160" s="24"/>
+      <c r="G160" s="24"/>
+      <c r="H160" s="24"/>
+      <c r="I160" s="24"/>
+      <c r="J160" s="24"/>
+      <c r="K160" s="24"/>
+      <c r="L160" s="24"/>
+      <c r="M160" s="24"/>
+    </row>
+    <row r="161" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A161" s="24"/>
+      <c r="B161" s="24"/>
+      <c r="C161" s="24"/>
+      <c r="D161" s="24"/>
+      <c r="E161" s="24"/>
+      <c r="F161" s="24"/>
+      <c r="G161" s="24"/>
+      <c r="H161" s="24"/>
+      <c r="I161" s="24"/>
+      <c r="J161" s="24"/>
+      <c r="K161" s="24"/>
+      <c r="L161" s="24"/>
+      <c r="M161" s="24"/>
+    </row>
+    <row r="162" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A162" s="24"/>
+      <c r="B162" s="24"/>
+      <c r="C162" s="24"/>
+      <c r="D162" s="24"/>
+      <c r="E162" s="24"/>
+      <c r="F162" s="24"/>
+      <c r="G162" s="24"/>
+      <c r="H162" s="24"/>
+      <c r="I162" s="24"/>
+      <c r="J162" s="24"/>
+      <c r="K162" s="24"/>
+      <c r="L162" s="24"/>
+      <c r="M162" s="24"/>
+    </row>
+    <row r="163" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A163" s="24"/>
+      <c r="B163" s="24"/>
+      <c r="C163" s="24"/>
+      <c r="D163" s="24"/>
+      <c r="E163" s="24"/>
+      <c r="F163" s="24"/>
+      <c r="G163" s="24"/>
+      <c r="H163" s="24"/>
+      <c r="I163" s="24"/>
+      <c r="J163" s="24"/>
+      <c r="K163" s="24"/>
+      <c r="L163" s="24"/>
+      <c r="M163" s="24"/>
+    </row>
+    <row r="164" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A164" s="24"/>
+      <c r="B164" s="24"/>
+      <c r="C164" s="24"/>
+      <c r="D164" s="24"/>
+      <c r="E164" s="24"/>
+      <c r="F164" s="24"/>
+      <c r="G164" s="24"/>
+      <c r="H164" s="24"/>
+      <c r="I164" s="24"/>
+      <c r="J164" s="24"/>
+      <c r="K164" s="24"/>
+      <c r="L164" s="24"/>
+      <c r="M164" s="24"/>
+    </row>
+    <row r="165" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A165" s="24"/>
+      <c r="B165" s="24"/>
+      <c r="C165" s="24"/>
+      <c r="D165" s="24"/>
+      <c r="E165" s="24"/>
+      <c r="F165" s="24"/>
+      <c r="G165" s="24"/>
+      <c r="H165" s="24"/>
+      <c r="I165" s="24"/>
+      <c r="J165" s="24"/>
+      <c r="K165" s="24"/>
+      <c r="L165" s="24"/>
+      <c r="M165" s="24"/>
+    </row>
+    <row r="166" spans="1:13" s="23" customFormat="1" ht="19" x14ac:dyDescent="0.25">
+      <c r="A166" s="24"/>
+      <c r="B166" s="24"/>
+      <c r="C166" s="24"/>
+      <c r="D166" s="24"/>
+      <c r="E166" s="24"/>
+      <c r="F166" s="24"/>
+      <c r="G166" s="24"/>
+      <c r="H166" s="24"/>
+      <c r="I166" s="24"/>
+      <c r="J166" s="24"/>
+      <c r="K166" s="24"/>
+      <c r="L166" s="24"/>
+      <c r="M166" s="24"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>